<commit_message>
delete the excel file after has been converted to pdf. layout refactoring
</commit_message>
<xml_diff>
--- a/invoice_template.xlsx
+++ b/invoice_template.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedaziz/workspace/personal_workspace/python_projects/factuur_azizcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794EF7B3-A247-2C4D-B4A9-6604EEE9A057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE91663-FEEF-554D-A1D5-FF3E5CBB6C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="500" windowWidth="37260" windowHeight="27400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="760" windowWidth="27640" windowHeight="18840" xr2:uid="{35C77A91-238D-FA4F-9276-78C2CD0D8742}"/>
   </bookViews>
   <sheets>
-    <sheet name="Factuur" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -61,17 +64,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00_-;[Red]&quot;€&quot;\ #,##0.00\-"/>
-    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00_-;[Red]&quot;€&quot;\ #,##0.00\-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -94,6 +105,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -102,23 +119,6 @@
       <b/>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -136,28 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -241,31 +220,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="dotted">
-        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
@@ -304,130 +260,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="42">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,6 +412,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2527299</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB2E6CEF-7CD2-6448-AF67-36C19BEC1C8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="165100" y="228600"/>
+          <a:ext cx="2539999" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,39 +762,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C735-292F-D740-AB6C-5D23DAC20244}">
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -795,318 +800,303 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="43"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C25" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D25" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E25" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26" t="str">
-        <f>IF(C22&gt;0,C22*D22," ")</f>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13" t="str">
+        <f>IF(C26&gt;0,C26*D26," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="7"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="10" t="str">
-        <f>IF(C23&gt;0,C23*D23," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17" t="str">
-        <f>IF(C24&gt;0,C24*D24," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="7"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="29" t="str">
-        <f>IF(C22&gt;0,C22*(D25)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="7"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="32"/>
-    </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17" t="str">
+      <c r="B27" s="33"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16" t="str">
         <f>IF(C27&gt;0,C27*D27," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17" t="str">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20" t="str">
         <f>IF(C28&gt;0,C28*D28," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="7" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21" t="str">
-        <f>IF(C29&gt;0,C29*D29," ")</f>
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="23" t="str">
+        <f>IF(C26&gt;0,C26*(D29)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="44" t="s">
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="37"/>
+    </row>
+    <row r="31" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20" t="str">
+        <f>IF(C31&gt;0,C31*D31," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20" t="str">
+        <f>IF(C32&gt;0,C32*D32," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27" t="str">
+        <f>IF(C33&gt;0,C33*D33," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="38" t="e">
-        <f>E22-E25</f>
+      <c r="D34" s="41"/>
+      <c r="E34" s="29" t="e">
+        <f>E26-E29</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="44" t="s">
+    <row r="35" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="39" t="e">
-        <f>E30*21%</f>
+      <c r="D35" s="39"/>
+      <c r="E35" s="30" t="e">
+        <f>E34*21%</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="37"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="37"/>
-    </row>
-    <row r="34" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="40"/>
-    </row>
-    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="45"/>
-      <c r="E35" s="36" t="e">
-        <f>E30+E31</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="31"/>
+    </row>
+    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="1"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="38"/>
+    </row>
+    <row r="39" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="C39" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="40"/>
+      <c r="E39" s="32" t="e">
+        <f>E34+E35</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C35:D35"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B22:E23 B25:B26">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(B22))&gt;0</formula>
+  <conditionalFormatting sqref="B26:E27 B29:B30">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(B26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="D29">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(D25))&gt;0</formula>
+      <formula>LEN(TRIM(D29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change name of the invoice file
</commit_message>
<xml_diff>
--- a/invoice_template.xlsx
+++ b/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedaziz/workspace/personal_workspace/python_projects/factuur_azizcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE91663-FEEF-554D-A1D5-FF3E5CBB6C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83408554-FBAA-B34E-AEFA-850B65383AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="760" windowWidth="27640" windowHeight="18840" xr2:uid="{35C77A91-238D-FA4F-9276-78C2CD0D8742}"/>
   </bookViews>
@@ -765,16 +765,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C735-292F-D740-AB6C-5D23DAC20244}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1"/>
     <col min="3" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>